<commit_message>
Busy merging Michelle's mockup with my real site.
</commit_message>
<xml_diff>
--- a/spreadsheet/Hollard Branch List 20170820 1100.xlsx
+++ b/spreadsheet/Hollard Branch List 20170820 1100.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -2523,7 +2524,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>